<commit_message>
Update database final BBB 23
</commit_message>
<xml_diff>
--- a/data/bbb_instagram.xlsx
+++ b/data/bbb_instagram.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BP23"/>
+  <dimension ref="A1:BQ23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -774,6 +774,11 @@
           <t>2023-04-24</t>
         </is>
       </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>2023-04-28</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -980,7 +985,10 @@
         <v>804916</v>
       </c>
       <c r="BP2" t="n">
-        <v>803334</v>
+        <v>802297</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>817325</v>
       </c>
     </row>
     <row r="3">
@@ -1188,7 +1196,10 @@
         <v>999663</v>
       </c>
       <c r="BP3" t="n">
-        <v>995611</v>
+        <v>994148</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>1003178</v>
       </c>
     </row>
     <row r="4">
@@ -1396,7 +1407,10 @@
         <v>1802127</v>
       </c>
       <c r="BP4" t="n">
-        <v>1911941</v>
+        <v>1939992</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>2282896</v>
       </c>
     </row>
     <row r="5">
@@ -1604,7 +1618,10 @@
         <v>1441790</v>
       </c>
       <c r="BP5" t="n">
-        <v>1454247</v>
+        <v>1452796</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>1426117</v>
       </c>
     </row>
     <row r="6">
@@ -1812,7 +1829,10 @@
         <v>4655395</v>
       </c>
       <c r="BP6" t="n">
-        <v>4656942</v>
+        <v>4656640</v>
+      </c>
+      <c r="BQ6" t="n">
+        <v>4797634</v>
       </c>
     </row>
     <row r="7">
@@ -2020,7 +2040,10 @@
         <v>1700798</v>
       </c>
       <c r="BP7" t="n">
-        <v>1698599</v>
+        <v>1692118</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>1696101</v>
       </c>
     </row>
     <row r="8">
@@ -2228,7 +2251,10 @@
         <v>11339319</v>
       </c>
       <c r="BP8" t="n">
-        <v>11353249</v>
+        <v>11355904</v>
+      </c>
+      <c r="BQ8" t="n">
+        <v>11466746</v>
       </c>
     </row>
     <row r="9">
@@ -2436,7 +2462,10 @@
         <v>2676810</v>
       </c>
       <c r="BP9" t="n">
-        <v>2687328</v>
+        <v>2714332</v>
+      </c>
+      <c r="BQ9" t="n">
+        <v>2945892</v>
       </c>
     </row>
     <row r="10">
@@ -2644,7 +2673,10 @@
         <v>1127937</v>
       </c>
       <c r="BP10" t="n">
-        <v>1153936</v>
+        <v>1155275</v>
+      </c>
+      <c r="BQ10" t="n">
+        <v>1227897</v>
       </c>
     </row>
     <row r="11">
@@ -2852,7 +2884,10 @@
         <v>1656390</v>
       </c>
       <c r="BP11" t="n">
-        <v>1670686</v>
+        <v>1674776</v>
+      </c>
+      <c r="BQ11" t="n">
+        <v>1724755</v>
       </c>
     </row>
     <row r="12">
@@ -3060,7 +3095,10 @@
         <v>2214662</v>
       </c>
       <c r="BP12" t="n">
-        <v>2216317</v>
+        <v>2215071</v>
+      </c>
+      <c r="BQ12" t="n">
+        <v>2359622</v>
       </c>
     </row>
     <row r="13">
@@ -3268,7 +3306,10 @@
         <v>1122936</v>
       </c>
       <c r="BP13" t="n">
-        <v>1144258</v>
+        <v>1146497</v>
+      </c>
+      <c r="BQ13" t="n">
+        <v>1225727</v>
       </c>
     </row>
     <row r="14">
@@ -3476,7 +3517,10 @@
         <v>1247414</v>
       </c>
       <c r="BP14" t="n">
-        <v>1251641</v>
+        <v>1250117</v>
+      </c>
+      <c r="BQ14" t="n">
+        <v>1274353</v>
       </c>
     </row>
     <row r="15">
@@ -3684,7 +3728,10 @@
         <v>9885460</v>
       </c>
       <c r="BP15" t="n">
-        <v>9955530</v>
+        <v>9964544</v>
+      </c>
+      <c r="BQ15" t="n">
+        <v>10020517</v>
       </c>
     </row>
     <row r="16">
@@ -3892,7 +3939,10 @@
         <v>1286555</v>
       </c>
       <c r="BP16" t="n">
-        <v>1285939</v>
+        <v>1285398</v>
+      </c>
+      <c r="BQ16" t="n">
+        <v>1295615</v>
       </c>
     </row>
     <row r="17">
@@ -4100,7 +4150,10 @@
         <v>529885</v>
       </c>
       <c r="BP17" t="n">
-        <v>529141</v>
+        <v>528114</v>
+      </c>
+      <c r="BQ17" t="n">
+        <v>539895</v>
       </c>
     </row>
     <row r="18">
@@ -4308,7 +4361,10 @@
         <v>1723959</v>
       </c>
       <c r="BP18" t="n">
-        <v>1738690</v>
+        <v>1740493</v>
+      </c>
+      <c r="BQ18" t="n">
+        <v>1792203</v>
       </c>
     </row>
     <row r="19">
@@ -4516,7 +4572,10 @@
         <v>602927</v>
       </c>
       <c r="BP19" t="n">
-        <v>604192</v>
+        <v>603685</v>
+      </c>
+      <c r="BQ19" t="n">
+        <v>633193</v>
       </c>
     </row>
     <row r="20">
@@ -4724,7 +4783,10 @@
         <v>3472057</v>
       </c>
       <c r="BP20" t="n">
-        <v>3473381</v>
+        <v>3471629</v>
+      </c>
+      <c r="BQ20" t="n">
+        <v>3497906</v>
       </c>
     </row>
     <row r="21">
@@ -4932,7 +4994,10 @@
         <v>2393464</v>
       </c>
       <c r="BP21" t="n">
-        <v>2401125</v>
+        <v>2397168</v>
+      </c>
+      <c r="BQ21" t="n">
+        <v>2943599</v>
       </c>
     </row>
     <row r="22">
@@ -5140,7 +5205,10 @@
         <v>423046</v>
       </c>
       <c r="BP22" t="n">
-        <v>422654</v>
+        <v>421279</v>
+      </c>
+      <c r="BQ22" t="n">
+        <v>425913</v>
       </c>
     </row>
     <row r="23">
@@ -5348,7 +5416,10 @@
         <v>10272554</v>
       </c>
       <c r="BP23" t="n">
-        <v>10271080</v>
+        <v>10273671</v>
+      </c>
+      <c r="BQ23" t="n">
+        <v>10295867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: correção dados incorretos
</commit_message>
<xml_diff>
--- a/data/bbb_instagram.xlsx
+++ b/data/bbb_instagram.xlsx
@@ -461,14 +461,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Alane</t>
+          <t>Alane</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>373357</v>
       </c>
       <c r="D2" t="n">
-        <v>387408</v>
+        <v>373357</v>
       </c>
     </row>
     <row r="3">
@@ -477,14 +477,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Beatriz</t>
+          <t>Beatriz</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>219727</v>
       </c>
       <c r="D3" t="n">
-        <v>237960</v>
+        <v>219727</v>
       </c>
     </row>
     <row r="4">
@@ -493,14 +493,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Deniziane</t>
+          <t>Deniziane</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>93728</v>
       </c>
       <c r="D4" t="n">
-        <v>97957</v>
+        <v>93728</v>
       </c>
     </row>
     <row r="5">
@@ -509,14 +509,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fernanda</t>
+          <t>Fernanda</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>48703</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>48703</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -525,14 +525,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Giovanna</t>
+          <t>Giovanna</t>
         </is>
       </c>
       <c r="C6" t="n">
         <v>69811</v>
       </c>
       <c r="D6" t="n">
-        <v>71644</v>
+        <v>69811</v>
       </c>
     </row>
     <row r="7">
@@ -541,14 +541,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Leidy Elin</t>
+          <t>Leidy Elin</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>374737</v>
       </c>
       <c r="D7" t="n">
-        <v>378448</v>
+        <v>374737</v>
       </c>
     </row>
     <row r="8">
@@ -557,14 +557,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Lucas Luigi</t>
+          <t>Lucas Luigi</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>41727</v>
       </c>
       <c r="D8" t="n">
-        <v>45168</v>
+        <v>41727</v>
       </c>
     </row>
     <row r="9">
@@ -573,14 +573,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Lucas Pizane</t>
+          <t>Lucas Pizane</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>97110</v>
       </c>
       <c r="D9" t="n">
-        <v>105726</v>
+        <v>97110</v>
       </c>
     </row>
     <row r="10">
@@ -589,14 +589,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Marcus</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>78515</v>
       </c>
       <c r="D10" t="n">
-        <v>81815</v>
+        <v>78515</v>
       </c>
     </row>
     <row r="11">
@@ -605,14 +605,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Matteus</t>
+          <t>Matteus</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>71936</v>
       </c>
       <c r="D11" t="n">
-        <v>76815</v>
+        <v>71936</v>
       </c>
     </row>
     <row r="12">
@@ -621,14 +621,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Maycon</t>
+          <t>Maycon</t>
         </is>
       </c>
       <c r="C12" t="n">
         <v>56925</v>
       </c>
       <c r="D12" t="n">
-        <v>56606</v>
+        <v>56925</v>
       </c>
     </row>
     <row r="13">
@@ -637,14 +637,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mc Bin Laden</t>
+          <t>Mc Bin Laden</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>3876068</v>
       </c>
       <c r="D13" t="n">
-        <v>3894549</v>
+        <v>3876068</v>
       </c>
     </row>
     <row r="14">
@@ -653,14 +653,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Nizam</t>
+          <t>Nizam</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>59532</v>
       </c>
       <c r="D14" t="n">
-        <v>65201</v>
+        <v>59532</v>
       </c>
     </row>
     <row r="15">
@@ -669,14 +669,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rodriguinho</t>
+          <t>Rodriguinho</t>
         </is>
       </c>
       <c r="C15" t="n">
         <v>2204265</v>
       </c>
       <c r="D15" t="n">
-        <v>2212854</v>
+        <v>2204265</v>
       </c>
     </row>
     <row r="16">
@@ -685,14 +685,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Vanessa Lopes</t>
+          <t>Vanessa Lopes</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>13973281</v>
       </c>
       <c r="D16" t="n">
-        <v>14017258</v>
+        <v>13973281</v>
       </c>
     </row>
     <row r="17">
@@ -701,14 +701,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Vinicius Rodrigues</t>
+          <t>Vinicius Rodrigues</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>71472</v>
       </c>
       <c r="D17" t="n">
-        <v>83919</v>
+        <v>71472</v>
       </c>
     </row>
     <row r="18">
@@ -717,14 +717,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Wanessa Camargo</t>
+          <t>Wanessa Camargo</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>4213058</v>
       </c>
       <c r="D18" t="n">
-        <v>4230709</v>
+        <v>4213058</v>
       </c>
     </row>
     <row r="19">
@@ -733,14 +733,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Yasmin Brunet</t>
+          <t>Yasmin Brunet</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>4788293</v>
       </c>
       <c r="D19" t="n">
-        <v>4832531</v>
+        <v>4788293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: atualizaçao de membros bbb
</commit_message>
<xml_diff>
--- a/data/bbb_instagram.xlsx
+++ b/data/bbb_instagram.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,6 @@
           <t>2024-01-08</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2024-01-09</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -465,10 +460,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>373357</v>
-      </c>
-      <c r="D2" t="n">
-        <v>373357</v>
+        <v>466633</v>
       </c>
     </row>
     <row r="3">
@@ -481,10 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>219727</v>
-      </c>
-      <c r="D3" t="n">
-        <v>219727</v>
+        <v>312266</v>
       </c>
     </row>
     <row r="4">
@@ -497,10 +486,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>93728</v>
-      </c>
-      <c r="D4" t="n">
-        <v>93728</v>
+        <v>247702</v>
       </c>
     </row>
     <row r="5">
@@ -513,10 +499,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
+        <v>57154</v>
       </c>
     </row>
     <row r="6">
@@ -525,14 +508,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Giovanna</t>
+          <t>Giovanna Pitel</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>69811</v>
-      </c>
-      <c r="D6" t="n">
-        <v>69811</v>
+        <v>73873</v>
       </c>
     </row>
     <row r="7">
@@ -545,10 +525,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>374737</v>
-      </c>
-      <c r="D7" t="n">
-        <v>374737</v>
+        <v>389503</v>
       </c>
     </row>
     <row r="8">
@@ -561,10 +538,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>41727</v>
-      </c>
-      <c r="D8" t="n">
-        <v>41727</v>
+        <v>48937</v>
       </c>
     </row>
     <row r="9">
@@ -577,10 +551,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>97110</v>
-      </c>
-      <c r="D9" t="n">
-        <v>97110</v>
+        <v>132462</v>
       </c>
     </row>
     <row r="10">
@@ -593,10 +564,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>78515</v>
-      </c>
-      <c r="D10" t="n">
-        <v>78515</v>
+        <v>95898</v>
       </c>
     </row>
     <row r="11">
@@ -609,10 +577,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>71936</v>
-      </c>
-      <c r="D11" t="n">
-        <v>71936</v>
+        <v>146109</v>
       </c>
     </row>
     <row r="12">
@@ -625,10 +590,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>56925</v>
-      </c>
-      <c r="D12" t="n">
-        <v>56925</v>
+        <v>52695</v>
       </c>
     </row>
     <row r="13">
@@ -641,10 +603,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3876068</v>
-      </c>
-      <c r="D13" t="n">
-        <v>3876068</v>
+        <v>3980296</v>
       </c>
     </row>
     <row r="14">
@@ -657,10 +616,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>59532</v>
-      </c>
-      <c r="D14" t="n">
-        <v>59532</v>
+        <v>79928</v>
       </c>
     </row>
     <row r="15">
@@ -673,10 +629,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2204265</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2204265</v>
+        <v>2231638</v>
       </c>
     </row>
     <row r="16">
@@ -689,10 +642,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>13973281</v>
-      </c>
-      <c r="D16" t="n">
-        <v>13973281</v>
+        <v>14154533</v>
       </c>
     </row>
     <row r="17">
@@ -705,10 +655,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>71472</v>
-      </c>
-      <c r="D17" t="n">
-        <v>71472</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
@@ -721,10 +668,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4213058</v>
-      </c>
-      <c r="D18" t="n">
-        <v>4213058</v>
+        <v>4323681</v>
       </c>
     </row>
     <row r="19">
@@ -737,10 +681,111 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4788293</v>
-      </c>
-      <c r="D19" t="n">
-        <v>4788293</v>
+        <v>5270698</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Davi</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>292415</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Giovanna</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>201669</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Isabelle</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>614226</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Juninho</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>21799</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Lucas Henrique</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>38615</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Michel</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>25078</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Raqueli</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>90877</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Thalyta</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>29370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>